<commit_message>
update: README.md file; document-API.xlsx. install: -D @types/node
</commit_message>
<xml_diff>
--- a/document-API.xlsx
+++ b/document-API.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspace\shop_backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspace\express-base-with-typescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5805CDC-6CA2-4BB4-BDF2-2174590F277A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F216CDFF-7DEC-482E-B2A8-2BBE1AE18AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Validation" sheetId="10" r:id="rId1"/>
     <sheet name="Update Note" sheetId="3" r:id="rId2"/>
     <sheet name="Library List" sheetId="2" r:id="rId3"/>
-    <sheet name="API List" sheetId="9" r:id="rId4"/>
+    <sheet name="Error List" sheetId="11" r:id="rId4"/>
+    <sheet name="API List" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="89">
   <si>
     <t>The library name</t>
   </si>
@@ -182,9 +183,6 @@
     <t>^0.25.10</t>
   </si>
   <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
     <t>Update sheet(s)</t>
   </si>
   <si>
@@ -237,6 +235,88 @@
   </si>
   <si>
     <t>- Library List</t>
+  </si>
+  <si>
+    <t>The Error Information</t>
+  </si>
+  <si>
+    <t>Api Name</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Status Code</t>
+  </si>
+  <si>
+    <t>Error Code</t>
+  </si>
+  <si>
+    <t>Error Message</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Error Description</t>
+  </si>
+  <si>
+    <t>@types/node</t>
+  </si>
+  <si>
+    <t>^24.5.2</t>
+  </si>
+  <si>
+    <t>Document Status</t>
+  </si>
+  <si>
+    <t>Working Status</t>
+  </si>
+  <si>
+    <t>NOT UPDATED</t>
+  </si>
+  <si>
+    <t>NOT START YET</t>
+  </si>
+  <si>
+    <t>NEWLY UPDATED</t>
+  </si>
+  <si>
+    <t>INPROGRESS</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Creation Date</t>
+  </si>
+  <si>
+    <t>Updation Date</t>
+  </si>
+  <si>
+    <t>- Data Validation
+- Library List
+- API List
+- Error List</t>
+  </si>
+  <si>
+    <t>- Create Error List sheet.
+- Update Data Validation, Library List, API List</t>
+  </si>
+  <si>
+    <t>Mothod</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
   </si>
 </sst>
 </file>
@@ -306,7 +386,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,8 +410,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -442,12 +528,225 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -479,68 +778,176 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -823,70 +1230,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1CF79B-1D3A-4B43-8F36-00089404C517}">
-  <dimension ref="B2:B12"/>
+  <dimension ref="B2:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="D5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="H6" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="H7" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -899,7 +1350,7 @@
   <dimension ref="C2:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+      <selection activeCell="C3" sqref="C3:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,72 +1360,72 @@
   <sheetData>
     <row r="2" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="18"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="15"/>
     </row>
     <row r="4" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="21"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="18"/>
     </row>
     <row r="6" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22" t="s">
+      <c r="D6" s="19"/>
+      <c r="E6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="O6" s="24"/>
-      <c r="P6" s="22" t="s">
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="22"/>
+      <c r="P6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" s="22"/>
-    </row>
-    <row r="7" spans="3:17" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q6" s="19"/>
+    </row>
+    <row r="7" spans="3:17" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="20" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="8"/>
@@ -985,22 +1436,22 @@
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
-      <c r="N7" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="O7" s="15"/>
+      <c r="N7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="12"/>
       <c r="P7" s="9">
         <v>45866</v>
       </c>
       <c r="Q7" s="10"/>
     </row>
-    <row r="8" spans="3:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="11" t="s">
-        <v>62</v>
+      <c r="E8" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -1010,19 +1461,23 @@
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="O8" s="13"/>
-      <c r="P8" s="9" t="s">
-        <v>32</v>
+      <c r="N8" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" s="33"/>
+      <c r="P8" s="9">
+        <v>45918</v>
       </c>
       <c r="Q8" s="10"/>
     </row>
-    <row r="9" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
+    <row r="9" spans="3:17" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
+      <c r="E9" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -1031,9 +1486,13 @@
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="9"/>
+      <c r="N9" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="O9" s="24"/>
+      <c r="P9" s="9">
+        <v>45920</v>
+      </c>
       <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1048,8 +1507,8 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="15"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="12"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="10"/>
     </row>
@@ -1065,8 +1524,8 @@
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="15"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="12"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="10"/>
     </row>
@@ -1082,8 +1541,8 @@
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="15"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="12"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="10"/>
     </row>
@@ -1099,8 +1558,8 @@
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="15"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="12"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="10"/>
     </row>
@@ -1116,8 +1575,8 @@
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="15"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="12"/>
       <c r="P14" s="9"/>
       <c r="Q14" s="10"/>
     </row>
@@ -1133,8 +1592,8 @@
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="15"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="12"/>
       <c r="P15" s="9"/>
       <c r="Q15" s="10"/>
     </row>
@@ -1150,8 +1609,8 @@
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="15"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="12"/>
       <c r="P16" s="9"/>
       <c r="Q16" s="10"/>
     </row>
@@ -1167,8 +1626,8 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="15"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="12"/>
       <c r="P17" s="9"/>
       <c r="Q17" s="10"/>
     </row>
@@ -1184,8 +1643,8 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="15"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="12"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="10"/>
     </row>
@@ -1201,8 +1660,8 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="15"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="12"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="10"/>
     </row>
@@ -1218,8 +1677,8 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="15"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="12"/>
       <c r="P20" s="9"/>
       <c r="Q20" s="10"/>
     </row>
@@ -1235,8 +1694,8 @@
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="15"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="12"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="10"/>
     </row>
@@ -1252,8 +1711,8 @@
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="15"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="12"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="10"/>
     </row>
@@ -1269,8 +1728,8 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="15"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="12"/>
       <c r="P23" s="9"/>
       <c r="Q23" s="10"/>
     </row>
@@ -1286,8 +1745,8 @@
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="15"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="12"/>
       <c r="P24" s="9"/>
       <c r="Q24" s="10"/>
     </row>
@@ -1303,8 +1762,8 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="15"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="12"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="10"/>
     </row>
@@ -1320,8 +1779,8 @@
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="15"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="12"/>
       <c r="P26" s="9"/>
       <c r="Q26" s="10"/>
     </row>
@@ -1337,8 +1796,8 @@
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="15"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="12"/>
       <c r="P27" s="9"/>
       <c r="Q27" s="10"/>
     </row>
@@ -1354,8 +1813,8 @@
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="15"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="12"/>
       <c r="P28" s="9"/>
       <c r="Q28" s="10"/>
     </row>
@@ -1371,8 +1830,8 @@
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="15"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="12"/>
       <c r="P29" s="9"/>
       <c r="Q29" s="10"/>
     </row>
@@ -1388,8 +1847,8 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="15"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="12"/>
       <c r="P30" s="9"/>
       <c r="Q30" s="10"/>
     </row>
@@ -1405,8 +1864,8 @@
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="15"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="12"/>
       <c r="P31" s="9"/>
       <c r="Q31" s="10"/>
     </row>
@@ -1422,8 +1881,8 @@
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="15"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="12"/>
       <c r="P32" s="9"/>
       <c r="Q32" s="10"/>
     </row>
@@ -1439,8 +1898,8 @@
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="15"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="12"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="10"/>
     </row>
@@ -1456,8 +1915,8 @@
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="15"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="12"/>
       <c r="P34" s="9"/>
       <c r="Q34" s="10"/>
     </row>
@@ -1473,13 +1932,114 @@
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="15"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="12"/>
       <c r="P35" s="9"/>
       <c r="Q35" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="121">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:M10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:M11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:M12"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:M8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="C3:Q4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:M6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="E7:M7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:M9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:M13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:M14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:M15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:M16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:M17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:M18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:M19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:M20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:M21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:M22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:M23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:M24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:M25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:M26"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:M27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:M28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:M29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:M30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="N30:O30"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="E34:M34"/>
     <mergeCell ref="P34:Q34"/>
@@ -1500,107 +2060,6 @@
     <mergeCell ref="P33:Q33"/>
     <mergeCell ref="N32:O32"/>
     <mergeCell ref="N33:O33"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:M28"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:M29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:M30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:M25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:M26"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:M27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:M22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:M23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:M24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:M19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:M20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:M21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:M16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:M17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:M18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:M13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:M14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:M15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="C3:Q4"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:M6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="E7:M7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:M9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:M10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:M11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:M12"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:M8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="N12:O12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1620,10 +2079,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2262A8F-CB71-4CEC-A967-D0CE8749E9E1}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="C2:R37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21:M21"/>
+      <selection activeCell="C3" sqref="C3:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,67 +2101,67 @@
       </c>
     </row>
     <row r="3" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
       <c r="R3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
       <c r="R4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="3:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22" t="s">
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22" t="s">
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22" t="s">
+      <c r="K6" s="19"/>
+      <c r="L6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22" t="s">
+      <c r="M6" s="19"/>
+      <c r="N6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="O6" s="22"/>
+      <c r="O6" s="19"/>
     </row>
     <row r="7" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="8" t="s">
@@ -1713,21 +2175,21 @@
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
-      <c r="J7" s="30" t="s">
+      <c r="J7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="30"/>
+      <c r="K7" s="29"/>
       <c r="L7" s="26">
         <v>45866</v>
       </c>
       <c r="M7" s="27"/>
       <c r="N7" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O7" s="7"/>
     </row>
     <row r="8" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="28" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="8"/>
@@ -1747,7 +2209,7 @@
       </c>
       <c r="M8" s="27"/>
       <c r="N8" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O8" s="7"/>
     </row>
@@ -1772,7 +2234,7 @@
       </c>
       <c r="M9" s="27"/>
       <c r="N9" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O9" s="7"/>
     </row>
@@ -1797,7 +2259,7 @@
       </c>
       <c r="M10" s="27"/>
       <c r="N10" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O10" s="7"/>
     </row>
@@ -1822,7 +2284,7 @@
       </c>
       <c r="M11" s="27"/>
       <c r="N11" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O11" s="7"/>
     </row>
@@ -1838,21 +2300,21 @@
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="30" t="s">
+      <c r="J12" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="30"/>
+      <c r="K12" s="29"/>
       <c r="L12" s="26">
         <v>45866</v>
       </c>
       <c r="M12" s="27"/>
       <c r="N12" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O12" s="7"/>
     </row>
     <row r="13" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="28" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="8"/>
@@ -1872,7 +2334,7 @@
       </c>
       <c r="M13" s="27"/>
       <c r="N13" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O13" s="7"/>
     </row>
@@ -1888,21 +2350,21 @@
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="30" t="s">
+      <c r="J14" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="30"/>
+      <c r="K14" s="29"/>
       <c r="L14" s="26">
         <v>45866</v>
       </c>
       <c r="M14" s="27"/>
       <c r="N14" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O14" s="7"/>
     </row>
     <row r="15" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="28" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="8"/>
@@ -1922,12 +2384,12 @@
       </c>
       <c r="M15" s="27"/>
       <c r="N15" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O15" s="7"/>
     </row>
     <row r="16" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="28" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="8"/>
@@ -1947,12 +2409,12 @@
       </c>
       <c r="M16" s="27"/>
       <c r="N16" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O16" s="7"/>
     </row>
     <row r="17" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="28" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="8"/>
@@ -1972,12 +2434,12 @@
       </c>
       <c r="M17" s="27"/>
       <c r="N17" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O17" s="7"/>
     </row>
     <row r="18" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="28" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="8"/>
@@ -1997,12 +2459,12 @@
       </c>
       <c r="M18" s="27"/>
       <c r="N18" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O18" s="7"/>
     </row>
     <row r="19" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="28" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="8"/>
@@ -2022,12 +2484,12 @@
       </c>
       <c r="M19" s="27"/>
       <c r="N19" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O19" s="7"/>
     </row>
     <row r="20" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="28" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="8"/>
@@ -2047,7 +2509,7 @@
       </c>
       <c r="M20" s="27"/>
       <c r="N20" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O20" s="7"/>
     </row>
@@ -2072,7 +2534,7 @@
       </c>
       <c r="M21" s="27"/>
       <c r="N21" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O21" s="7"/>
     </row>
@@ -2097,7 +2559,7 @@
       </c>
       <c r="M22" s="27"/>
       <c r="N22" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O22" s="7"/>
     </row>
@@ -2122,24 +2584,34 @@
       </c>
       <c r="M23" s="27"/>
       <c r="N23" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O23" s="7"/>
     </row>
     <row r="24" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="8"/>
+      <c r="C24" s="28" t="s">
+        <v>70</v>
+      </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="G24" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
+      <c r="J24" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="K24" s="8"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
+      <c r="L24" s="25">
+        <v>45920</v>
+      </c>
+      <c r="M24" s="25"/>
+      <c r="N24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="O24" s="7"/>
     </row>
     <row r="25" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="8"/>
@@ -2151,10 +2623,10 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
     </row>
     <row r="26" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="8"/>
@@ -2166,10 +2638,10 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
     </row>
     <row r="27" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="8"/>
@@ -2181,10 +2653,10 @@
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
     </row>
     <row r="28" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="8"/>
@@ -2196,10 +2668,10 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
     </row>
     <row r="29" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="8"/>
@@ -2211,10 +2683,10 @@
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
     </row>
     <row r="30" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="8"/>
@@ -2226,10 +2698,10 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
     </row>
     <row r="31" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="8"/>
@@ -2241,10 +2713,10 @@
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
     </row>
     <row r="32" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="8"/>
@@ -2256,10 +2728,10 @@
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
     </row>
     <row r="33" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="8"/>
@@ -2271,10 +2743,10 @@
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
     </row>
     <row r="34" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="8"/>
@@ -2286,10 +2758,10 @@
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
     </row>
     <row r="35" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="8"/>
@@ -2301,10 +2773,10 @@
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
-      <c r="L35" s="28"/>
-      <c r="M35" s="28"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
     </row>
     <row r="36" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="8"/>
@@ -2316,10 +2788,10 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="28"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
     </row>
     <row r="37" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="8"/>
@@ -2331,13 +2803,154 @@
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
+      <c r="L37" s="25"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="161">
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="C3:O4"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="N33:O33"/>
     <mergeCell ref="C34:F34"/>
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="J34:K34"/>
@@ -2358,236 +2971,1422 @@
     <mergeCell ref="J36:K36"/>
     <mergeCell ref="L36:M36"/>
     <mergeCell ref="N36:O36"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="C3:O4"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:K37" xr:uid="{01552295-EEDD-438D-B306-8A908509B898}">
       <formula1>$R$3:$R$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0037F603-5C6C-4C3F-981E-39026A8A7D21}">
+          <x14:formula1>
+            <xm:f>'Data Validation'!$B$3:$B$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>N7:O37</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E4BB31-5B58-4293-A48C-57028B521C10}">
-  <dimension ref="C2:R37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A778BA8E-4115-43B6-A4EF-28A16ADC5255}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="B1:AA38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="B2" sqref="B2:AA4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="9" width="5.85546875" customWidth="1"/>
+    <col min="10" max="11" width="6.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="15"/>
+    </row>
+    <row r="3" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="60"/>
+      <c r="AA3" s="61"/>
+    </row>
+    <row r="4" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="18"/>
+    </row>
+    <row r="5" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="34"/>
+      <c r="AA5" s="34"/>
+    </row>
+    <row r="6" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="37"/>
+      <c r="J6" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" s="37"/>
+      <c r="L6" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="36"/>
+      <c r="Y6" s="40"/>
+      <c r="Z6" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="40"/>
+    </row>
+    <row r="7" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="48"/>
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="49"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+    </row>
+    <row r="8" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="55"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="55"/>
+      <c r="V8" s="55"/>
+      <c r="W8" s="55"/>
+      <c r="X8" s="55"/>
+      <c r="Y8" s="56"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+    </row>
+    <row r="9" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="55"/>
+      <c r="S9" s="55"/>
+      <c r="T9" s="55"/>
+      <c r="U9" s="55"/>
+      <c r="V9" s="55"/>
+      <c r="W9" s="55"/>
+      <c r="X9" s="55"/>
+      <c r="Y9" s="56"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+    </row>
+    <row r="10" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="55"/>
+      <c r="S10" s="55"/>
+      <c r="T10" s="55"/>
+      <c r="U10" s="55"/>
+      <c r="V10" s="55"/>
+      <c r="W10" s="55"/>
+      <c r="X10" s="55"/>
+      <c r="Y10" s="56"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+    </row>
+    <row r="11" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="55"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="55"/>
+      <c r="S11" s="55"/>
+      <c r="T11" s="55"/>
+      <c r="U11" s="55"/>
+      <c r="V11" s="55"/>
+      <c r="W11" s="55"/>
+      <c r="X11" s="55"/>
+      <c r="Y11" s="56"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+    </row>
+    <row r="12" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="55"/>
+      <c r="P12" s="55"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="55"/>
+      <c r="S12" s="55"/>
+      <c r="T12" s="55"/>
+      <c r="U12" s="55"/>
+      <c r="V12" s="55"/>
+      <c r="W12" s="55"/>
+      <c r="X12" s="55"/>
+      <c r="Y12" s="56"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+    </row>
+    <row r="13" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="50"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="55"/>
+      <c r="S13" s="55"/>
+      <c r="T13" s="55"/>
+      <c r="U13" s="55"/>
+      <c r="V13" s="55"/>
+      <c r="W13" s="55"/>
+      <c r="X13" s="55"/>
+      <c r="Y13" s="56"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+    </row>
+    <row r="14" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="55"/>
+      <c r="S14" s="55"/>
+      <c r="T14" s="55"/>
+      <c r="U14" s="55"/>
+      <c r="V14" s="55"/>
+      <c r="W14" s="55"/>
+      <c r="X14" s="55"/>
+      <c r="Y14" s="56"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+    </row>
+    <row r="15" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="55"/>
+      <c r="T15" s="55"/>
+      <c r="U15" s="55"/>
+      <c r="V15" s="55"/>
+      <c r="W15" s="55"/>
+      <c r="X15" s="55"/>
+      <c r="Y15" s="56"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+    </row>
+    <row r="16" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="55"/>
+      <c r="S16" s="55"/>
+      <c r="T16" s="55"/>
+      <c r="U16" s="55"/>
+      <c r="V16" s="55"/>
+      <c r="W16" s="55"/>
+      <c r="X16" s="55"/>
+      <c r="Y16" s="56"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+    </row>
+    <row r="17" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="55"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="55"/>
+      <c r="S17" s="55"/>
+      <c r="T17" s="55"/>
+      <c r="U17" s="55"/>
+      <c r="V17" s="55"/>
+      <c r="W17" s="55"/>
+      <c r="X17" s="55"/>
+      <c r="Y17" s="56"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+    </row>
+    <row r="18" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="55"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="55"/>
+      <c r="S18" s="55"/>
+      <c r="T18" s="55"/>
+      <c r="U18" s="55"/>
+      <c r="V18" s="55"/>
+      <c r="W18" s="55"/>
+      <c r="X18" s="55"/>
+      <c r="Y18" s="56"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+    </row>
+    <row r="19" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="55"/>
+      <c r="T19" s="55"/>
+      <c r="U19" s="55"/>
+      <c r="V19" s="55"/>
+      <c r="W19" s="55"/>
+      <c r="X19" s="55"/>
+      <c r="Y19" s="56"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+    </row>
+    <row r="20" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="55"/>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="55"/>
+      <c r="T20" s="55"/>
+      <c r="U20" s="55"/>
+      <c r="V20" s="55"/>
+      <c r="W20" s="55"/>
+      <c r="X20" s="55"/>
+      <c r="Y20" s="56"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+    </row>
+    <row r="21" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="50"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="55"/>
+      <c r="S21" s="55"/>
+      <c r="T21" s="55"/>
+      <c r="U21" s="55"/>
+      <c r="V21" s="55"/>
+      <c r="W21" s="55"/>
+      <c r="X21" s="55"/>
+      <c r="Y21" s="56"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
+    </row>
+    <row r="22" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="50"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="55"/>
+      <c r="S22" s="55"/>
+      <c r="T22" s="55"/>
+      <c r="U22" s="55"/>
+      <c r="V22" s="55"/>
+      <c r="W22" s="55"/>
+      <c r="X22" s="55"/>
+      <c r="Y22" s="56"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="7"/>
+    </row>
+    <row r="23" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="50"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="55"/>
+      <c r="S23" s="55"/>
+      <c r="T23" s="55"/>
+      <c r="U23" s="55"/>
+      <c r="V23" s="55"/>
+      <c r="W23" s="55"/>
+      <c r="X23" s="55"/>
+      <c r="Y23" s="56"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
+    </row>
+    <row r="24" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="55"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="55"/>
+      <c r="T24" s="55"/>
+      <c r="U24" s="55"/>
+      <c r="V24" s="55"/>
+      <c r="W24" s="55"/>
+      <c r="X24" s="55"/>
+      <c r="Y24" s="56"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
+    </row>
+    <row r="25" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="50"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="55"/>
+      <c r="S25" s="55"/>
+      <c r="T25" s="55"/>
+      <c r="U25" s="55"/>
+      <c r="V25" s="55"/>
+      <c r="W25" s="55"/>
+      <c r="X25" s="55"/>
+      <c r="Y25" s="56"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+    </row>
+    <row r="26" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="54"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="55"/>
+      <c r="T26" s="55"/>
+      <c r="U26" s="55"/>
+      <c r="V26" s="55"/>
+      <c r="W26" s="55"/>
+      <c r="X26" s="55"/>
+      <c r="Y26" s="56"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7"/>
+    </row>
+    <row r="27" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="50"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="55"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="55"/>
+      <c r="P27" s="55"/>
+      <c r="Q27" s="54"/>
+      <c r="R27" s="55"/>
+      <c r="S27" s="55"/>
+      <c r="T27" s="55"/>
+      <c r="U27" s="55"/>
+      <c r="V27" s="55"/>
+      <c r="W27" s="55"/>
+      <c r="X27" s="55"/>
+      <c r="Y27" s="56"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7"/>
+    </row>
+    <row r="28" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="50"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="54"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="55"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="55"/>
+      <c r="T28" s="55"/>
+      <c r="U28" s="55"/>
+      <c r="V28" s="55"/>
+      <c r="W28" s="55"/>
+      <c r="X28" s="55"/>
+      <c r="Y28" s="56"/>
+      <c r="Z28" s="7"/>
+      <c r="AA28" s="7"/>
+    </row>
+    <row r="29" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="50"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="55"/>
+      <c r="Q29" s="54"/>
+      <c r="R29" s="55"/>
+      <c r="S29" s="55"/>
+      <c r="T29" s="55"/>
+      <c r="U29" s="55"/>
+      <c r="V29" s="55"/>
+      <c r="W29" s="55"/>
+      <c r="X29" s="55"/>
+      <c r="Y29" s="56"/>
+      <c r="Z29" s="7"/>
+      <c r="AA29" s="7"/>
+    </row>
+    <row r="30" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="50"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="55"/>
+      <c r="N30" s="55"/>
+      <c r="O30" s="55"/>
+      <c r="P30" s="55"/>
+      <c r="Q30" s="54"/>
+      <c r="R30" s="55"/>
+      <c r="S30" s="55"/>
+      <c r="T30" s="55"/>
+      <c r="U30" s="55"/>
+      <c r="V30" s="55"/>
+      <c r="W30" s="55"/>
+      <c r="X30" s="55"/>
+      <c r="Y30" s="56"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="7"/>
+    </row>
+    <row r="31" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="55"/>
+      <c r="N31" s="55"/>
+      <c r="O31" s="55"/>
+      <c r="P31" s="55"/>
+      <c r="Q31" s="54"/>
+      <c r="R31" s="55"/>
+      <c r="S31" s="55"/>
+      <c r="T31" s="55"/>
+      <c r="U31" s="55"/>
+      <c r="V31" s="55"/>
+      <c r="W31" s="55"/>
+      <c r="X31" s="55"/>
+      <c r="Y31" s="56"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="7"/>
+    </row>
+    <row r="32" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="50"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="54"/>
+      <c r="M32" s="55"/>
+      <c r="N32" s="55"/>
+      <c r="O32" s="55"/>
+      <c r="P32" s="55"/>
+      <c r="Q32" s="54"/>
+      <c r="R32" s="55"/>
+      <c r="S32" s="55"/>
+      <c r="T32" s="55"/>
+      <c r="U32" s="55"/>
+      <c r="V32" s="55"/>
+      <c r="W32" s="55"/>
+      <c r="X32" s="55"/>
+      <c r="Y32" s="56"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="7"/>
+    </row>
+    <row r="33" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="50"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="52"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="54"/>
+      <c r="M33" s="55"/>
+      <c r="N33" s="55"/>
+      <c r="O33" s="55"/>
+      <c r="P33" s="55"/>
+      <c r="Q33" s="54"/>
+      <c r="R33" s="55"/>
+      <c r="S33" s="55"/>
+      <c r="T33" s="55"/>
+      <c r="U33" s="55"/>
+      <c r="V33" s="55"/>
+      <c r="W33" s="55"/>
+      <c r="X33" s="55"/>
+      <c r="Y33" s="56"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7"/>
+    </row>
+    <row r="34" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="50"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="54"/>
+      <c r="M34" s="55"/>
+      <c r="N34" s="55"/>
+      <c r="O34" s="55"/>
+      <c r="P34" s="55"/>
+      <c r="Q34" s="54"/>
+      <c r="R34" s="55"/>
+      <c r="S34" s="55"/>
+      <c r="T34" s="55"/>
+      <c r="U34" s="55"/>
+      <c r="V34" s="55"/>
+      <c r="W34" s="55"/>
+      <c r="X34" s="55"/>
+      <c r="Y34" s="56"/>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="7"/>
+    </row>
+    <row r="35" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="50"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="54"/>
+      <c r="M35" s="55"/>
+      <c r="N35" s="55"/>
+      <c r="O35" s="55"/>
+      <c r="P35" s="55"/>
+      <c r="Q35" s="54"/>
+      <c r="R35" s="55"/>
+      <c r="S35" s="55"/>
+      <c r="T35" s="55"/>
+      <c r="U35" s="55"/>
+      <c r="V35" s="55"/>
+      <c r="W35" s="55"/>
+      <c r="X35" s="55"/>
+      <c r="Y35" s="56"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+    </row>
+    <row r="36" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="50"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="54"/>
+      <c r="M36" s="55"/>
+      <c r="N36" s="55"/>
+      <c r="O36" s="55"/>
+      <c r="P36" s="55"/>
+      <c r="Q36" s="54"/>
+      <c r="R36" s="55"/>
+      <c r="S36" s="55"/>
+      <c r="T36" s="55"/>
+      <c r="U36" s="55"/>
+      <c r="V36" s="55"/>
+      <c r="W36" s="55"/>
+      <c r="X36" s="55"/>
+      <c r="Y36" s="56"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="7"/>
+    </row>
+    <row r="37" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="50"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="54"/>
+      <c r="M37" s="55"/>
+      <c r="N37" s="55"/>
+      <c r="O37" s="55"/>
+      <c r="P37" s="55"/>
+      <c r="Q37" s="54"/>
+      <c r="R37" s="55"/>
+      <c r="S37" s="55"/>
+      <c r="T37" s="55"/>
+      <c r="U37" s="55"/>
+      <c r="V37" s="55"/>
+      <c r="W37" s="55"/>
+      <c r="X37" s="55"/>
+      <c r="Y37" s="56"/>
+      <c r="Z37" s="7"/>
+      <c r="AA37" s="7"/>
+    </row>
+    <row r="38" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="50"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="52"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="53"/>
+      <c r="L38" s="54"/>
+      <c r="M38" s="55"/>
+      <c r="N38" s="55"/>
+      <c r="O38" s="55"/>
+      <c r="P38" s="55"/>
+      <c r="Q38" s="54"/>
+      <c r="R38" s="55"/>
+      <c r="S38" s="55"/>
+      <c r="T38" s="55"/>
+      <c r="U38" s="55"/>
+      <c r="V38" s="55"/>
+      <c r="W38" s="55"/>
+      <c r="X38" s="55"/>
+      <c r="Y38" s="56"/>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="199">
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:P38"/>
+    <mergeCell ref="Q38:Y38"/>
+    <mergeCell ref="Z38:AA38"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:P37"/>
+    <mergeCell ref="Q37:Y37"/>
+    <mergeCell ref="Z37:AA37"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="L36:P36"/>
+    <mergeCell ref="Q36:Y36"/>
+    <mergeCell ref="Z36:AA36"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:P35"/>
+    <mergeCell ref="Q35:Y35"/>
+    <mergeCell ref="Z35:AA35"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:P34"/>
+    <mergeCell ref="Q34:Y34"/>
+    <mergeCell ref="Z34:AA34"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:P33"/>
+    <mergeCell ref="Q33:Y33"/>
+    <mergeCell ref="Z33:AA33"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:P32"/>
+    <mergeCell ref="Q32:Y32"/>
+    <mergeCell ref="Z32:AA32"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:P31"/>
+    <mergeCell ref="Q31:Y31"/>
+    <mergeCell ref="Z31:AA31"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:P30"/>
+    <mergeCell ref="Q30:Y30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:P29"/>
+    <mergeCell ref="Q29:Y29"/>
+    <mergeCell ref="Z29:AA29"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:P28"/>
+    <mergeCell ref="Q28:Y28"/>
+    <mergeCell ref="Z28:AA28"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:P27"/>
+    <mergeCell ref="Q27:Y27"/>
+    <mergeCell ref="Z27:AA27"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:P26"/>
+    <mergeCell ref="Q26:Y26"/>
+    <mergeCell ref="Z26:AA26"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:P25"/>
+    <mergeCell ref="Q25:Y25"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:P24"/>
+    <mergeCell ref="Q24:Y24"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:P23"/>
+    <mergeCell ref="Q23:Y23"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:P22"/>
+    <mergeCell ref="Q22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:P21"/>
+    <mergeCell ref="Q21:Y21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:P20"/>
+    <mergeCell ref="Q20:Y20"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:P19"/>
+    <mergeCell ref="Q19:Y19"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:P18"/>
+    <mergeCell ref="Q18:Y18"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:P17"/>
+    <mergeCell ref="Q17:Y17"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:P16"/>
+    <mergeCell ref="Q16:Y16"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:P15"/>
+    <mergeCell ref="Q15:Y15"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:P14"/>
+    <mergeCell ref="Q14:Y14"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="Q13:Y13"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:P12"/>
+    <mergeCell ref="Q12:Y12"/>
+    <mergeCell ref="Z12:AA12"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:P11"/>
+    <mergeCell ref="Q11:Y11"/>
+    <mergeCell ref="Z11:AA11"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:P10"/>
+    <mergeCell ref="Q10:Y10"/>
+    <mergeCell ref="Z10:AA10"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:P9"/>
+    <mergeCell ref="Q9:Y9"/>
+    <mergeCell ref="Z9:AA9"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="Q8:Y8"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="Q7:Y7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:P6"/>
+    <mergeCell ref="Q6:Y6"/>
+    <mergeCell ref="B2:AA4"/>
+  </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2242DBF1-FABE-4EEA-8B3A-EF2BAE64C9EF}">
+          <x14:formula1>
+            <xm:f>'Data Validation'!$B$3:$B$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>Z7:AA38</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4C0F2130-4734-4C1C-A673-47BAE36536DE}">
+          <x14:formula1>
+            <xm:f>'Data Validation'!$H$3:$H$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>G7:G38</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E4BB31-5B58-4293-A48C-57028B521C10}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="C2:V37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="10" max="11" width="10" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" customWidth="1"/>
+    <col min="14" max="17" width="9.28515625" customWidth="1"/>
+    <col min="22" max="22" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="R2" s="4"/>
-    </row>
-    <row r="3" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="R3" s="4"/>
-    </row>
-    <row r="4" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="R4" s="5"/>
-    </row>
-    <row r="6" spans="3:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="22" t="s">
+    <row r="2" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V2" s="4"/>
+    </row>
+    <row r="3" spans="3:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="64"/>
+      <c r="V3" s="4"/>
+    </row>
+    <row r="4" spans="3:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
+      <c r="S4" s="67"/>
+      <c r="V4" s="5"/>
+    </row>
+    <row r="6" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C6" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22" t="s">
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="O6" s="22"/>
-    </row>
-    <row r="7" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S6" s="19"/>
+    </row>
+    <row r="7" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -2601,9 +4400,13 @@
       <c r="M7" s="27"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
-    </row>
-    <row r="8" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="25"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+    </row>
+    <row r="8" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="28"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -2616,8 +4419,12 @@
       <c r="M8" s="27"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
-    </row>
-    <row r="9" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+    </row>
+    <row r="9" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -2627,12 +4434,16 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
-    </row>
-    <row r="10" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+    </row>
+    <row r="10" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -2646,8 +4457,12 @@
       <c r="M10" s="27"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
-    </row>
-    <row r="11" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+    </row>
+    <row r="11" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -2661,8 +4476,12 @@
       <c r="M11" s="27"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+    </row>
+    <row r="12" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -2672,13 +4491,17 @@
       <c r="I12" s="8"/>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
-    </row>
-    <row r="13" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="25"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+    </row>
+    <row r="13" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="28"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -2691,8 +4514,12 @@
       <c r="M13" s="27"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
-    </row>
-    <row r="14" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+    </row>
+    <row r="14" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -2706,9 +4533,13 @@
       <c r="M14" s="27"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
-    </row>
-    <row r="15" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="25"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+    </row>
+    <row r="15" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="28"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -2717,13 +4548,17 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
-    </row>
-    <row r="16" spans="3:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="25"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+    </row>
+    <row r="16" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="28"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -2732,13 +4567,17 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
-    </row>
-    <row r="17" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="25"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+    </row>
+    <row r="17" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="28"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -2747,13 +4586,17 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
-    </row>
-    <row r="18" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="25"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+    </row>
+    <row r="18" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="28"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -2762,13 +4605,17 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
-    </row>
-    <row r="19" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="25"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+    </row>
+    <row r="19" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="28"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -2777,13 +4624,17 @@
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
-    </row>
-    <row r="20" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="25"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+    </row>
+    <row r="20" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="28"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -2792,12 +4643,16 @@
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
-    </row>
-    <row r="21" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+    </row>
+    <row r="21" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -2807,12 +4662,16 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
-    </row>
-    <row r="22" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+    </row>
+    <row r="22" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -2822,12 +4681,16 @@
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
-    </row>
-    <row r="23" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+    </row>
+    <row r="23" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -2837,12 +4700,16 @@
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
-    </row>
-    <row r="24" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+    </row>
+    <row r="24" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -2852,12 +4719,16 @@
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-    </row>
-    <row r="25" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+    </row>
+    <row r="25" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -2867,12 +4738,16 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-    </row>
-    <row r="26" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+    </row>
+    <row r="26" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -2882,12 +4757,16 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-    </row>
-    <row r="27" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+    </row>
+    <row r="27" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -2897,12 +4776,16 @@
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-    </row>
-    <row r="28" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+    </row>
+    <row r="28" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -2912,12 +4795,16 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-    </row>
-    <row r="29" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+    </row>
+    <row r="29" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -2927,12 +4814,16 @@
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-    </row>
-    <row r="30" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+    </row>
+    <row r="30" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -2942,12 +4833,16 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-    </row>
-    <row r="31" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+    </row>
+    <row r="31" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -2957,12 +4852,16 @@
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-    </row>
-    <row r="32" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+    </row>
+    <row r="32" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -2972,12 +4871,16 @@
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-    </row>
-    <row r="33" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+    </row>
+    <row r="33" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
@@ -2987,12 +4890,16 @@
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-    </row>
-    <row r="34" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+    </row>
+    <row r="34" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -3002,12 +4909,16 @@
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-    </row>
-    <row r="35" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+    </row>
+    <row r="35" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -3017,12 +4928,16 @@
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
-      <c r="L35" s="28"/>
-      <c r="M35" s="28"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-    </row>
-    <row r="36" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+    </row>
+    <row r="36" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -3032,12 +4947,16 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="28"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-    </row>
-    <row r="37" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+    </row>
+    <row r="37" spans="3:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -3047,181 +4966,273 @@
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
+      <c r="L37" s="25"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="161">
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="G34:I34"/>
+  <mergeCells count="225">
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="C3:S4"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="R32:S32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="R33:S33"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:I34"/>
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="L34:M34"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="F37:I37"/>
     <mergeCell ref="J37:K37"/>
     <mergeCell ref="L37:M37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:I35"/>
     <mergeCell ref="J35:K35"/>
     <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="R35:S35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="F36:I36"/>
     <mergeCell ref="J36:K36"/>
     <mergeCell ref="L36:M36"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="C3:O4"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="P37:Q37"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:K37" xr:uid="{91C91B20-81C8-476F-8BA1-79218BF1E0B5}">
-      <formula1>$R$3:$R$4</formula1>
+      <formula1>$V$3:$V$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D6667D53-BB68-4491-838F-27FD68EA81C8}">
+          <x14:formula1>
+            <xm:f>'Data Validation'!$B$3:$B$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>R7:S37</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9F68A650-A343-4F7E-8990-C9544985EAB8}">
+          <x14:formula1>
+            <xm:f>'Data Validation'!$D$3:$D$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>N7:O37</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{977E5F4F-EC80-4611-AE6C-139DC42D1A78}">
+          <x14:formula1>
+            <xm:f>'Data Validation'!$F$3:$F$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>P7:Q37</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>